<commit_message>
Version 0 Mixed integer deployment at refineries, starting the modeling
</commit_message>
<xml_diff>
--- a/LCOH_ANRs.xlsx
+++ b/LCOH_ANRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A920FC-C58F-5447-A1D3-39CD83242DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E560BA8-BC30-C342-B1F8-2FD9E17BC0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="500" windowWidth="19080" windowHeight="23500" activeTab="5" xr2:uid="{C3A9BDD3-7070-B24E-8B62-0D3AA983BDBB}"/>
+    <workbookView xWindow="37340" yWindow="500" windowWidth="17580" windowHeight="21920" activeTab="4" xr2:uid="{C3A9BDD3-7070-B24E-8B62-0D3AA983BDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="ANRs" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
   <si>
     <t>Reactor</t>
   </si>
@@ -148,9 +148,6 @@
     <t>HTSE/SOEC</t>
   </si>
   <si>
-    <t>https://www.osti.gov/biblio/1867883</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
     <t xml:space="preserve">Capacity </t>
   </si>
   <si>
-    <t>HTSE total electric demand (33% eff.)</t>
-  </si>
-  <si>
     <t>MWh-e/kg-H2</t>
   </si>
   <si>
@@ -359,6 +353,105 @@
   </si>
   <si>
     <t>kg/h</t>
+  </si>
+  <si>
+    <t>Hunter et al</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>$/MWh (2018)</t>
+  </si>
+  <si>
+    <t>HHV efficiency</t>
+  </si>
+  <si>
+    <t>HHV hydrogen</t>
+  </si>
+  <si>
+    <t>kWh/kg</t>
+  </si>
+  <si>
+    <t>Electric demand</t>
+  </si>
+  <si>
+    <t>$/MWe (2018)</t>
+  </si>
+  <si>
+    <t>$/MWe-year (2018)</t>
+  </si>
+  <si>
+    <t>kg-H2/h</t>
+  </si>
+  <si>
+    <t>Jang et al</t>
+  </si>
+  <si>
+    <t>Eff (LHV)</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Lazard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAPEX </t>
+  </si>
+  <si>
+    <t>$/MWe</t>
+  </si>
+  <si>
+    <t>OPEX excl. elec</t>
+  </si>
+  <si>
+    <t>Production rate</t>
+  </si>
+  <si>
+    <t>kg-H2/MWe-y</t>
+  </si>
+  <si>
+    <t>kg-H2/MWh-e</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>$/MW-y</t>
+  </si>
+  <si>
+    <t>$/y</t>
+  </si>
+  <si>
+    <t>VOM excl. energy costs</t>
+  </si>
+  <si>
+    <t>$/MWh</t>
+  </si>
+  <si>
+    <t>Ruth</t>
+  </si>
+  <si>
+    <t>Rabiti</t>
+  </si>
+  <si>
+    <t>$/kW</t>
+  </si>
+  <si>
+    <t>Electricity demand</t>
+  </si>
+  <si>
+    <t>Thermal demand</t>
+  </si>
+  <si>
+    <t>MWh-th/kg</t>
+  </si>
+  <si>
+    <t>MWh-e/kg</t>
   </si>
 </sst>
 </file>
@@ -668,34 +761,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.1196603620637178</c:v>
+                  <c:v>2.2881845957966989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4986475037099347</c:v>
+                  <c:v>2.6973032239695587</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.930687828961736</c:v>
+                  <c:v>3.1636930450452661</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3935687927858686</c:v>
+                  <c:v>3.6633754989260878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8728134517279438</c:v>
+                  <c:v>4.1807226484200948</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.3606031170209052</c:v>
+                  <c:v>4.7072941775614368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8530913240385036</c:v>
+                  <c:v>5.2389378073984556</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3484197138731986</c:v>
+                  <c:v>5.7736474296405023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8456452195821154</c:v>
+                  <c:v>6.3104049985241568</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.3442380105302307</c:v>
+                  <c:v>6.8486385590706202</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2939,7 +3032,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="4">
         <f>(ANRs!B13*1000*ANRs!B5*LCOe!$B$2 + ANRs!B14*1000*ANRs!B5 + (ANRs!B15+ANRs!B16)*ANRs!B5*(365*24)) / (ANRs!B5*LCOe!$A$8*(365*24))</f>
@@ -2964,7 +3057,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!B13*1000*'ANRs NOAK'!B5*LCOe!$B$2 + 'ANRs NOAK'!B14*1000*'ANRs NOAK'!B5 + ('ANRs NOAK'!B15+'ANRs NOAK'!B16)*'ANRs NOAK'!B5*(365*24)) / ('ANRs NOAK'!B5*(365*24)*LCOe!$A$8)</f>
@@ -2989,10 +3082,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3092,10 +3185,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18550AEC-35FC-FF41-BAD4-E0EA7304A6F8}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3104,114 +3197,181 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>1076</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B4">
-        <v>1076</v>
+        <v>566</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B5">
-        <v>611</v>
+        <f>B4*1000/24</f>
+        <v>23583.333333333332</v>
       </c>
       <c r="C5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
-        <f>B5*1000/24</f>
-        <v>25458.333333333332</v>
-      </c>
-      <c r="C6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
+        <v>695620000</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="4">
+        <v>32617000</v>
+      </c>
+      <c r="C7" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="4">
-        <v>695620000</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="4">
-        <v>32617000</v>
+        <v>25992000</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="4">
+        <v>820</v>
+      </c>
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="5">
+        <v>3.6799999999999999E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4">
-        <v>25992000</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B14" s="5">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="5">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="D14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11">
-        <f>LCOH!B2*POWER(1+LCOH!B2,HTSE!B10)/(POWER(1+LCOH!B2,HTSE!B10)-1)</f>
+      <c r="B15">
+        <f>LCOH!B2*POWER(1+LCOH!B2,HTSE!B14)/(POWER(1+LCOH!B2,HTSE!B14)-1)</f>
         <v>0.10185220882315059</v>
       </c>
     </row>
@@ -3222,9 +3382,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926589E9-7BDE-6C47-8D87-520B9E9EBED4}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -3234,172 +3394,241 @@
     <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="B3">
         <v>35.299999999999997</v>
       </c>
       <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="B4">
         <v>9.5</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5">
         <v>624</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <f>B5*1000/24</f>
         <v>26000</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4">
         <v>423000</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4">
+        <f>B12*B5*1000*365</f>
+        <v>15943200.000000002</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="4">
+        <f>B12*365*24/B17</f>
+        <v>17218.189731422077</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="4">
+        <f>B13*1000*B5*365</f>
+        <v>10932480</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="4">
+        <f>B13/B17</f>
+        <v>1.3478035014811802</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="4">
-        <f>B10*B5*1000*365</f>
-        <v>15943200.000000002</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B12" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="4">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="5">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15">
+        <f>LCOH!B2*POWER(1+LCOH!B2,B14)/(POWER(1+LCOH!B2,B14)-1)</f>
+        <v>0.10185220882315059</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="4">
-        <f>B11*1000*B5*365</f>
-        <v>10932480</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B10" s="4">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" s="4">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="5">
-        <v>20</v>
-      </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13">
-        <f>LCOH!B2*POWER(1+LCOH!B2,B12)/(POWER(1+LCOH!B2,B12)-1)</f>
-        <v>0.10185220882315059</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B14">
-        <f>(B5*1000/24)*B15</f>
+      <c r="B16">
+        <f>(B5*1000/24)*B17</f>
         <v>925.95099999999979</v>
       </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17">
         <f>(B3+B4*0.033)/1000</f>
         <v>3.5613499999999992E-2</v>
       </c>
-      <c r="C15" t="s">
-        <v>100</v>
+      <c r="C17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D17" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3409,108 +3638,222 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29183C49-8C12-1942-B979-D0FAB5F16434}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3">
+        <v>65.75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>51</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5">
+        <v>743865</v>
+      </c>
+      <c r="G5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4">
         <f>920*B5*1000</f>
         <v>92000000</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F6">
+        <v>60020</v>
+      </c>
+      <c r="G6" t="s">
+        <v>119</v>
+      </c>
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>54</v>
       </c>
       <c r="B7">
         <v>18030</v>
       </c>
       <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F7">
+        <v>86488</v>
+      </c>
+      <c r="G7" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>121</v>
+      </c>
+      <c r="F8">
+        <f>F7/(364*24)</f>
+        <v>9.9001831501831496</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>56</v>
       </c>
       <c r="B9" s="4">
         <f>0.021*B7*1000</f>
         <v>378630</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="E9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9">
+        <f>1/F8</f>
+        <v>0.10100823235593377</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
+      </c>
+      <c r="H9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="4">
         <f>0.015*B6</f>
         <v>1380000</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3518,10 +3861,23 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11">
+        <f>F8*F4</f>
+        <v>990.01831501831498</v>
+      </c>
+      <c r="G11" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3537,10 +3893,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E909B9-6B9E-B548-A749-B6BC49AC0882}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3548,103 +3904,194 @@
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4">
+        <v>1500000</v>
+      </c>
+      <c r="H4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>51</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5">
+        <v>12800</v>
+      </c>
+      <c r="H5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4">
         <f>1190*B5*1000</f>
         <v>119000000</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6">
+        <v>1.3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>54</v>
       </c>
       <c r="B7">
         <v>17000</v>
       </c>
       <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>56</v>
       </c>
       <c r="B8" s="4">
         <f>0.021*B7*1000</f>
         <v>357000</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>108</v>
+      </c>
+      <c r="G8">
+        <v>39.4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" s="4">
         <f>0.015*B6</f>
         <v>1785000</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9">
+        <f>G8/(G7*1000)</f>
+        <v>5.4344827586206894E-2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10">
         <v>9.6999999999999993</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10">
+        <f>G3/G9</f>
+        <v>1840.1015228426397</v>
+      </c>
+      <c r="H10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -3652,10 +4099,10 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -3674,7 +4121,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3687,19 +4134,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" t="s">
-        <v>64</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
@@ -3710,36 +4157,36 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="8">
-        <f>HTSE!B7/HTSE!B4</f>
+        <f>HTSE!B6/HTSE!B3</f>
         <v>646486.98884758365</v>
       </c>
       <c r="C2" s="8">
-        <f>HTSE!B8/HTSE!B4</f>
+        <f>HTSE!B7/HTSE!B3</f>
         <v>30313.197026022306</v>
       </c>
       <c r="D2" s="8">
-        <f>HTSE!B9/HTSE!B4</f>
+        <f>HTSE!B8/HTSE!B3</f>
         <v>24156.133828996284</v>
       </c>
       <c r="E2" s="7">
-        <f>HTSE!B5*1000*365/HTSE!B4</f>
-        <v>207263.01115241635</v>
+        <f>HTSE!B4*1000*365/HTSE!B3</f>
+        <v>191998.14126394052</v>
       </c>
       <c r="F2">
-        <f>HTSE!B11</f>
+        <f>HTSE!B15</f>
         <v>0.10185220882315059</v>
       </c>
       <c r="G2">
-        <f>HTSE!B10</f>
+        <f>HTSE!B14</f>
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B3" s="9">
         <f>Alkaline!B6/Alkaline!B5</f>
@@ -3768,7 +4215,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="8">
         <f>PEM!B6/PEM!B5</f>
@@ -3797,22 +4244,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="9">
         <f>'HTSE future'!B7</f>
         <v>423000</v>
       </c>
       <c r="C5" s="8">
-        <f>'HTSE future'!B8/'HTSE future'!B14</f>
+        <f>'HTSE future'!B8/'HTSE future'!B16</f>
         <v>17218.189731422081</v>
       </c>
       <c r="D5" s="8">
-        <f>'HTSE future'!B9/'HTSE future'!B14</f>
+        <f>'HTSE future'!B10/'HTSE future'!B16</f>
         <v>11806.758672975138</v>
       </c>
       <c r="E5" s="7">
-        <f>'HTSE future'!B5*365*1000/'HTSE future'!B14</f>
+        <f>'HTSE future'!B5*365*1000/'HTSE future'!B16</f>
         <v>245974.13902031537</v>
       </c>
       <c r="F5">
@@ -3848,58 +4295,58 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
         <v>68</v>
-      </c>
-      <c r="I1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2">
         <v>0.08</v>
       </c>
       <c r="I2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
         <v>71</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" t="s">
         <v>72</v>
       </c>
-      <c r="I3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>73</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>74</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>75</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>76</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>77</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>78</v>
-      </c>
-      <c r="P3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I4">
         <v>0.02</v>
@@ -3926,11 +4373,11 @@
       </c>
       <c r="O4">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P4">
         <f>(L4+M4+N4)/O4</f>
-        <v>2.1196603620637178</v>
+        <v>2.2881845957966989</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -3959,16 +4406,16 @@
       </c>
       <c r="O5">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P13" si="0">(L5+M5+N5)/O5</f>
-        <v>2.4986475037099347</v>
+        <v>2.6973032239695587</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6">
         <v>0.06</v>
@@ -3995,16 +4442,16 @@
       </c>
       <c r="O6">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>2.930687828961736</v>
+        <v>3.1636930450452661</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" t="str">
         <f>ANRs!B1</f>
@@ -4051,11 +4498,11 @@
       </c>
       <c r="O7">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>3.3935687927858686</v>
+        <v>3.6633754989260878</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -4065,23 +4512,23 @@
       </c>
       <c r="B8" s="6">
         <f>((ANRs!B$13*1000*ANRs!B$5*ANRs!B$19+ANRs!B$14*1000*ANRs!B$5+(ANRs!B$15+ANRs!B$16)*ANRs!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!B$5))/('H2 recap'!$E2*ANRs!B$5)</f>
-        <v>3.7051575231946456</v>
+        <v>3.9997371849327354</v>
       </c>
       <c r="C8" s="6">
         <f>((ANRs!C$13*1000*ANRs!C$5*ANRs!C$19+ANRs!C$14*1000*ANRs!C$5+(ANRs!C$15+ANRs!C$16)*ANRs!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!C$5))/('H2 recap'!$E2*ANRs!C$5)</f>
-        <v>4.8449555412155272</v>
+        <v>5.2301551867185276</v>
       </c>
       <c r="D8" s="6">
         <f>((ANRs!D$13*1000*ANRs!D$5*ANRs!D$19+ANRs!D$14*1000*ANRs!D$5+(ANRs!D$15+ANRs!D$16)*ANRs!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!D$5))/('H2 recap'!$E2*ANRs!D$5)</f>
-        <v>3.3935687927858682</v>
+        <v>3.6633754989260874</v>
       </c>
       <c r="E8" s="6">
         <f>((ANRs!E$13*1000*ANRs!E$5*ANRs!E$19+ANRs!E$14*1000*ANRs!E$5+(ANRs!E$15+ANRs!E$16)*ANRs!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!E$5))/('H2 recap'!$E2*ANRs!E$5)</f>
-        <v>3.0714591257602941</v>
+        <v>3.3156564060769256</v>
       </c>
       <c r="F8" s="6">
         <f>((ANRs!F$13*1000*ANRs!F$5*ANRs!F$19+ANRs!F$14*1000*ANRs!F$5+(ANRs!F$15+ANRs!F$16)*ANRs!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!F$5))/('H2 recap'!$E2*ANRs!F$5)</f>
-        <v>7.2116497339478816</v>
+        <v>7.7850141120886134</v>
       </c>
       <c r="I8">
         <v>0.1</v>
@@ -4108,11 +4555,11 @@
       </c>
       <c r="O8">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P8">
         <f t="shared" si="0"/>
-        <v>3.8728134517279438</v>
+        <v>4.1807226484200948</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
@@ -4165,11 +4612,11 @@
       </c>
       <c r="O9">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>4.3606031170209052</v>
+        <v>4.7072941775614368</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -4222,11 +4669,11 @@
       </c>
       <c r="O10">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>4.8530913240385036</v>
+        <v>5.2389378073984556</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -4279,11 +4726,11 @@
       </c>
       <c r="O11">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P11">
         <f t="shared" si="0"/>
-        <v>5.3484197138731986</v>
+        <v>5.7736474296405023</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
@@ -4312,22 +4759,22 @@
       </c>
       <c r="O12">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P12">
         <f t="shared" si="0"/>
-        <v>5.8456452195821154</v>
+        <v>6.3104049985241568</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
         <v>83</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>84</v>
-      </c>
-      <c r="C13" t="s">
-        <v>85</v>
       </c>
       <c r="I13">
         <v>0.2</v>
@@ -4354,16 +4801,16 @@
       </c>
       <c r="O13">
         <f>'H2 recap'!E$2*ANRs!D$5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="P13">
         <f t="shared" si="0"/>
-        <v>6.3442380105302307</v>
+        <v>6.8486385590706202</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <f>ANRs!D13*ANRs!D5*1000*ANRs!D19+'H2 recap'!B2*ANRs!D5*'H2 recap'!F2</f>
@@ -4376,7 +4823,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15">
         <f>ANRs!D14*ANRs!D5*1000+'H2 recap'!C2*ANRs!D5</f>
@@ -4389,7 +4836,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16">
         <f>(ANRs!D15+ANRs!D16)*ANRs!D5*(365*24)+'H2 recap'!D2*ANRs!D5</f>
@@ -4402,11 +4849,11 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B17">
         <f>'H2 recap'!E2*ANRs!D5</f>
-        <v>16581040.892193308</v>
+        <v>15359851.301115241</v>
       </c>
       <c r="C17">
         <f>'H2 recap'!E4*ANRs!E5</f>
@@ -4415,11 +4862,11 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <f>(B14+B15+B16)/B17</f>
-        <v>3.3935687927858686</v>
+        <v>3.6633754989260878</v>
       </c>
       <c r="C18">
         <f>(C14+C15+C16)/C17</f>
@@ -4428,12 +4875,12 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" t="str">
         <f>'ANRs NOAK'!B1</f>
@@ -4463,23 +4910,23 @@
       </c>
       <c r="B22" s="6">
         <f>(('ANRs NOAK'!B$13*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!B$5))/('H2 recap'!$E2*'ANRs NOAK'!B$5)</f>
-        <v>3.1873034471545294</v>
+        <v>3.4407109650378396</v>
       </c>
       <c r="C22" s="6">
         <f>(('ANRs NOAK'!C$13*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!C$5))/('H2 recap'!$E2*'ANRs NOAK'!C$5)</f>
-        <v>4.1432562511882685</v>
+        <v>4.472667083879915</v>
       </c>
       <c r="D22" s="6">
         <f>(('ANRs NOAK'!D$13*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!D$5))/('H2 recap'!$E2*'ANRs NOAK'!D$5)</f>
-        <v>2.9660935853012624</v>
+        <v>3.2019137466768046</v>
       </c>
       <c r="E22" s="6">
         <f>(('ANRs NOAK'!E$13*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!E$5))/('H2 recap'!$E2*'ANRs NOAK'!E$5)</f>
-        <v>2.6887055530267592</v>
+        <v>2.9024718955818902</v>
       </c>
       <c r="F22" s="6">
         <f>(('ANRs NOAK'!F$13*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!F$5))/('H2 recap'!$E2*'ANRs NOAK'!F$5)</f>
-        <v>5.9258715053105329</v>
+        <v>6.3970096991956451</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cost parametes for h2 techin summary
</commit_message>
<xml_diff>
--- a/LCOH_ANRs.xlsx
+++ b/LCOH_ANRs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/Library/CloudStorage/OneDrive-IdahoNationalLaboratory/Documents/Research/Hydrogen from Nuclear/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E560BA8-BC30-C342-B1F8-2FD9E17BC0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A088A028-3682-4F46-899A-B686186E204A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37340" yWindow="500" windowWidth="17580" windowHeight="21920" activeTab="4" xr2:uid="{C3A9BDD3-7070-B24E-8B62-0D3AA983BDBB}"/>
+    <workbookView xWindow="37340" yWindow="500" windowWidth="17580" windowHeight="21920" activeTab="7" xr2:uid="{C3A9BDD3-7070-B24E-8B62-0D3AA983BDBB}"/>
   </bookViews>
   <sheets>
     <sheet name="ANRs" sheetId="2" r:id="rId1"/>
@@ -3188,7 +3188,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3332,7 +3332,10 @@
       <c r="A12" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="4"/>
+      <c r="B12" s="4">
+        <f>B7/B3</f>
+        <v>30313.197026022306</v>
+      </c>
       <c r="C12" t="s">
         <v>125</v>
       </c>
@@ -3344,7 +3347,10 @@
       <c r="A13" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="4">
+        <f>B8/(B3*24*365)</f>
+        <v>2.7575495238580232</v>
+      </c>
       <c r="C13" t="s">
         <v>128</v>
       </c>
@@ -3384,8 +3390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926589E9-7BDE-6C47-8D87-520B9E9EBED4}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4120,8 +4126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1776E7-CBAE-9E47-8B69-07E0825574D9}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update lcoh calculations, fix learning rates calculations
</commit_message>
<xml_diff>
--- a/LCOH_ANRs.xlsx
+++ b/LCOH_ANRs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\H2_ANRs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49323FE1-0336-479B-BE84-FBACAE5E7191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B43631-A348-41D4-8D56-5BF257FC4543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="8" xr2:uid="{C3A9BDD3-7070-B24E-8B62-0D3AA983BDBB}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="140">
   <si>
     <t>Reactor</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Vanatta</t>
   </si>
   <si>
-    <t>Learning rates</t>
-  </si>
-  <si>
     <t>Pesimistic</t>
   </si>
   <si>
@@ -452,6 +449,21 @@
   </si>
   <si>
     <t>MWh-e/kg</t>
+  </si>
+  <si>
+    <t>N (number of units already deployed)</t>
+  </si>
+  <si>
+    <t>Learning rates /CAPEX ($/kWe)</t>
+  </si>
+  <si>
+    <t>NOAK 3% learning rate</t>
+  </si>
+  <si>
+    <t>NOAK 7% learning rate</t>
+  </si>
+  <si>
+    <t>NOAK 10% learning rate</t>
   </si>
 </sst>
 </file>
@@ -507,7 +519,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -524,6 +536,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2315,23 +2330,23 @@
       </c>
       <c r="B19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,B18)/(POWER(1+LCOH!$B$2,B18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="C19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,C18)/(POWER(1+LCOH!$B$2,C18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="D19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,D18)/(POWER(1+LCOH!$B$2,D18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="E19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,E18)/(POWER(1+LCOH!$B$2,E18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="F19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,F18)/(POWER(1+LCOH!$B$2,F18)-1)</f>
-        <v>0.10185220882315059</v>
+        <v>9.9589020191458474E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
@@ -2349,15 +2364,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4ACCCEC-4125-4707-BB58-29DEFB1ACF98}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="30.6875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.5">
@@ -2678,24 +2694,24 @@
         <v>CAPEX ($/Kwe)</v>
       </c>
       <c r="B13" s="10">
-        <f>ANRs!B13*(1-'ANRs NOAK'!$B$23)</f>
-        <v>4206.6000000000004</v>
+        <f>ANRs!B13*POWER($B$22, LOG(1-$B$23,2))</f>
+        <v>2685.5020560646503</v>
       </c>
       <c r="C13" s="10">
-        <f>ANRs!C13*(1-'ANRs NOAK'!$B$23)</f>
-        <v>5700</v>
+        <f>ANRs!C13*POWER($B$22, LOG(1-$B$23,2))</f>
+        <v>3638.8916748843503</v>
       </c>
       <c r="D13" s="10">
-        <f>ANRs!D13*(1-'ANRs NOAK'!$B$23)</f>
-        <v>3472.44</v>
+        <f>ANRs!D13*POWER($B$22, LOG(1-$B$23,2))</f>
+        <v>2216.8128083395459</v>
       </c>
       <c r="E13" s="10">
-        <f>ANRs!E13*(1-'ANRs NOAK'!$B$23)</f>
-        <v>3109.16</v>
+        <f>ANRs!E13*POWER($B$22, LOG(1-$B$23,2))</f>
+        <v>1984.8941122602503</v>
       </c>
       <c r="F13" s="10">
-        <f>ANRs!F13*(1-'ANRs NOAK'!$B$23)</f>
-        <v>8285.52</v>
+        <f>ANRs!F13*POWER($B$22, LOG(1-$B$23,2))</f>
+        <v>5289.4929386118911</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.5">
@@ -2776,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A17" t="str">
         <f>ANRs!A17</f>
         <v>Start-up fixed cost ($/startup)</v>
@@ -2802,7 +2818,7 @@
         <v>3350</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A18" t="str">
         <f>ANRs!A18</f>
         <v>Lifetime</v>
@@ -2828,41 +2844,50 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A19" t="str">
         <f>ANRs!A19</f>
         <v>CRF</v>
       </c>
       <c r="B19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,B18)/(POWER(1+LCOH!$B$2,B18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="C19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,C18)/(POWER(1+LCOH!$B$2,C18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="D19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,D18)/(POWER(1+LCOH!$B$2,D18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="E19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,E18)/(POWER(1+LCOH!$B$2,E18)-1)</f>
-        <v>8.0797948763645655E-2</v>
+        <v>7.7909172717496755E-2</v>
       </c>
       <c r="F19">
         <f>LCOH!$B$2*POWER(1+LCOH!$B$2,F18)/(POWER(1+LCOH!$B$2,F18)-1)</f>
-        <v>0.10185220882315059</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.5">
+        <v>9.9589020191458474E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.5">
+        <f>B28</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2870,39 +2895,118 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A26" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
+      <c r="B27">
+        <v>0.03</v>
+      </c>
+      <c r="C27">
+        <f>ANRs!B$13*POWER($B$22, LOG(1-$B27,2))</f>
+        <v>4085.8985805721031</v>
+      </c>
+      <c r="D27">
+        <f>ANRs!C$13*POWER($B$22, LOG(1-$B27,2))</f>
+        <v>5536.4479411546108</v>
+      </c>
+      <c r="E27">
+        <f>ANRs!D$13*POWER($B$22, LOG(1-$B27,2))</f>
+        <v>3372.8040857513893</v>
+      </c>
+      <c r="F27">
+        <f>ANRs!E$13*POWER($B$22, LOG(1-$B27,2))</f>
+        <v>3019.9478036351352</v>
+      </c>
+      <c r="G27">
+        <f>ANRs!F$13*POWER($B$22, LOG(1-$B27,2))</f>
+        <v>8047.7807272623422</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
         <v>30</v>
       </c>
-      <c r="B26">
-        <v>-0.23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A27" t="s">
+      <c r="B28">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C28">
+        <f>ANRs!B$13*POWER($B$22, LOG(1-$B28,2))</f>
+        <v>2685.5020560646503</v>
+      </c>
+      <c r="D28">
+        <f>ANRs!C$13*POWER($B$22, LOG(1-$B28,2))</f>
+        <v>3638.8916748843503</v>
+      </c>
+      <c r="E28">
+        <f>ANRs!D$13*POWER($B$22, LOG(1-$B28,2))</f>
+        <v>2216.8128083395459</v>
+      </c>
+      <c r="F28">
+        <f>ANRs!E$13*POWER($B$22, LOG(1-$B28,2))</f>
+        <v>1984.8941122602503</v>
+      </c>
+      <c r="G28">
+        <f>ANRs!F$13*POWER($B$22, LOG(1-$B28,2))</f>
+        <v>5289.4929386118911</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
         <v>31</v>
       </c>
-      <c r="B27">
-        <v>0.108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28">
-        <v>0.24</v>
+      <c r="B29">
+        <v>0.1</v>
+      </c>
+      <c r="C29">
+        <f>ANRs!B$13*POWER($B$22, LOG(1-$B29,2))</f>
+        <v>1936.9051097966403</v>
+      </c>
+      <c r="D29">
+        <f>ANRs!C$13*POWER($B$22, LOG(1-$B29,2))</f>
+        <v>2624.5326691011387</v>
+      </c>
+      <c r="E29">
+        <f>ANRs!D$13*POWER($B$22, LOG(1-$B29,2))</f>
+        <v>1598.8653020164138</v>
+      </c>
+      <c r="F29">
+        <f>ANRs!E$13*POWER($B$22, LOG(1-$B29,2))</f>
+        <v>1431.5950865723678</v>
+      </c>
+      <c r="G29">
+        <f>ANRs!F$13*POWER($B$22, LOG(1-$B29,2))</f>
+        <v>3815.0206878054155</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A26:B26"/>
+  </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23" xr:uid="{E4D0258E-90CD-40B0-9FC4-A541E2011814}">
-      <formula1>$B$26:$B$28</formula1>
+      <formula1>$B$27:$B$29</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2974,7 +3078,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" s="4">
         <f>(ANRs!B13*1000*ANRs!B5*LCOe!$B$2 + ANRs!B14*1000*ANRs!B5 + (ANRs!B15+ANRs!B16)*ANRs!B5*(365*24)) / (ANRs!B5*LCOe!$A$8*(365*24))</f>
@@ -2999,35 +3103,35 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!B13*1000*'ANRs NOAK'!B5*LCOe!$B$2 + 'ANRs NOAK'!B14*1000*'ANRs NOAK'!B5 + ('ANRs NOAK'!B15+'ANRs NOAK'!B16)*'ANRs NOAK'!B5*(365*24)) / ('ANRs NOAK'!B5*(365*24)*LCOe!$A$8)</f>
-        <v>38.623567056337052</v>
+        <v>33.365348639029143</v>
       </c>
       <c r="C4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!C13*1000*'ANRs NOAK'!C5*LCOe!$B$2 + 'ANRs NOAK'!C14*1000*'ANRs NOAK'!C5 + ('ANRs NOAK'!C15+'ANRs NOAK'!C16)*'ANRs NOAK'!C5*(365*24)) / ('ANRs NOAK'!C5*(365*24)*LCOe!$A$8)</f>
-        <v>53.095097958074518</v>
+        <v>45.970140753050245</v>
       </c>
       <c r="D4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!D13*1000*'ANRs NOAK'!D5*LCOe!$B$2 + 'ANRs NOAK'!D14*1000*'ANRs NOAK'!D5 + ('ANRs NOAK'!D15+'ANRs NOAK'!D16)*'ANRs NOAK'!D5*(365*24)) / ('ANRs NOAK'!D5*(365*24)*LCOe!$A$8)</f>
-        <v>37.704282053852793</v>
+        <v>33.363758124552014</v>
       </c>
       <c r="E4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!E13*1000*'ANRs NOAK'!E5*LCOe!$B$2 + 'ANRs NOAK'!E14*1000*'ANRs NOAK'!E5 + ('ANRs NOAK'!E15+'ANRs NOAK'!E16)*'ANRs NOAK'!E5*(365*24)) / ('ANRs NOAK'!E5*(365*24)*LCOe!$A$8)</f>
-        <v>33.067076258947857</v>
+        <v>29.180649602180615</v>
       </c>
       <c r="F4" s="4">
         <f xml:space="preserve"> ( 'ANRs NOAK'!F13*1000*'ANRs NOAK'!F5*LCOe!$B$2 + 'ANRs NOAK'!F14*1000*'ANRs NOAK'!F5 + ('ANRs NOAK'!F15+'ANRs NOAK'!F16)*'ANRs NOAK'!F5*(365*24)) / ('ANRs NOAK'!F5*(365*24)*LCOe!$A$8)</f>
-        <v>60.36500314936734</v>
+        <v>50.008165356144062</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.5">
@@ -3130,7 +3234,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -3141,177 +3245,177 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>1076</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>566</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <f>B4*1000/24</f>
         <v>23583.333333333332</v>
       </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4">
         <v>695620000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4">
         <v>32617000</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="4">
         <v>25992000</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="4">
         <v>820</v>
       </c>
       <c r="C9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B10" s="5">
         <v>3.6799999999999999E-2</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="5">
         <v>1.6500000000000001E-2</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="4">
         <f>B7/B3</f>
         <v>30313.197026022306</v>
       </c>
       <c r="C12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4">
         <f>B8/(B3*24*365)</f>
         <v>2.7575495238580232</v>
       </c>
       <c r="C13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -3320,7 +3424,7 @@
       </c>
       <c r="B15">
         <f>LCOH!B2*POWER(1+LCOH!B2,HTSE!B14)/(POWER(1+LCOH!B2,HTSE!B14)-1)</f>
-        <v>0.10185220882315059</v>
+        <v>9.9589020191458474E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3344,200 +3448,200 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3">
         <v>35.299999999999997</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4">
         <v>9.5</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>624</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <f>B5*1000/24</f>
         <v>26000</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4">
         <v>423000</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="4">
         <f>B12*B5*1000*365</f>
         <v>15943200.000000002</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="4">
         <f>B12*365*24/B17</f>
         <v>17218.189731422077</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="4">
         <f>B13*1000*B5*365</f>
         <v>10932480</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B11" s="4">
         <f>B13/B17</f>
         <v>1.3478035014811802</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="4">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="5">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.5">
@@ -3546,37 +3650,37 @@
       </c>
       <c r="B15">
         <f>LCOH!B2*POWER(1+LCOH!B2,B14)/(POWER(1+LCOH!B2,B14)-1)</f>
-        <v>0.10185220882315059</v>
+        <v>9.9589020191458474E-2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16">
         <f>(B5*1000/24)*B17</f>
         <v>925.95099999999979</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17">
         <f>(B3+B4*0.033)/1000</f>
         <v>3.5613499999999992E-2</v>
       </c>
       <c r="C17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3604,189 +3708,189 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="E2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" t="s">
         <v>35</v>
       </c>
-      <c r="G2" t="s">
-        <v>36</v>
-      </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3">
         <v>65.75</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
       <c r="E4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F4">
         <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5">
         <v>743865</v>
       </c>
       <c r="G5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <f>920*B5*1000</f>
         <v>92000000</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6">
         <v>60020</v>
       </c>
       <c r="G6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>18030</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7">
         <v>86488</v>
       </c>
       <c r="G7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8">
         <f>F7/(364*24)</f>
         <v>9.9001831501831496</v>
       </c>
       <c r="G8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H8" t="s">
         <v>123</v>
-      </c>
-      <c r="H8" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="4">
         <f>0.021*B7*1000</f>
         <v>378630</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F9">
         <f>1/F8</f>
         <v>0.10100823235593377</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="4">
         <f>0.015*B6</f>
         <v>1380000</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
         <v>22</v>
@@ -3795,10 +3899,10 @@
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
@@ -3809,20 +3913,20 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F11">
         <f>F8*F4</f>
         <v>990.01831501831498</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
@@ -3831,7 +3935,7 @@
       </c>
       <c r="B12">
         <f>LCOH!B2*POWER(1+LCOH!B2,B11)/(POWER(1+LCOH!B2,B11)-1)</f>
-        <v>0.11682954493601999</v>
+        <v>0.11469825673487978</v>
       </c>
     </row>
   </sheetData>
@@ -3844,7 +3948,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -3857,186 +3961,186 @@
         <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" t="s">
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="F2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3">
         <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
         <v>48</v>
       </c>
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4">
         <v>1500000</v>
       </c>
       <c r="H4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>100</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5">
         <v>12800</v>
       </c>
       <c r="H5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="4">
         <f>1190*B5*1000</f>
         <v>119000000</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G6">
         <v>1.3</v>
       </c>
       <c r="H6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7">
         <v>17000</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G7">
         <v>0.72499999999999998</v>
       </c>
       <c r="H7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="4">
         <f>0.021*B7*1000</f>
         <v>357000</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G8">
         <v>39.4</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4">
         <f>0.015*B6</f>
         <v>1785000</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G9">
         <f>G8/(G7*1000)</f>
         <v>5.4344827586206894E-2</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10">
         <v>9.6999999999999993</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G10">
         <f>G3/G9</f>
         <v>1840.1015228426397</v>
       </c>
       <c r="H10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.5">
@@ -4047,7 +4151,7 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.5">
@@ -4056,7 +4160,7 @@
       </c>
       <c r="B12">
         <f>LCOH!B2*POWER(1+LCOH!B2,B11)/(POWER(1+LCOH!B2,B11)-1)</f>
-        <v>0.11682954493601999</v>
+        <v>0.11469825673487978</v>
       </c>
     </row>
   </sheetData>
@@ -4069,7 +4173,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4082,19 +4186,19 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>62</v>
-      </c>
-      <c r="E1" t="s">
-        <v>63</v>
       </c>
       <c r="F1" t="s">
         <v>23</v>
@@ -4105,7 +4209,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" s="8">
         <f>HTSE!B6/HTSE!B3</f>
@@ -4125,7 +4229,7 @@
       </c>
       <c r="F2">
         <f>HTSE!B15</f>
-        <v>0.10185220882315059</v>
+        <v>9.9589020191458474E-2</v>
       </c>
       <c r="G2">
         <f>HTSE!B14</f>
@@ -4134,7 +4238,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" s="9">
         <f>Alkaline!B6/Alkaline!B5</f>
@@ -4154,7 +4258,7 @@
       </c>
       <c r="F3">
         <f>Alkaline!B12</f>
-        <v>0.11682954493601999</v>
+        <v>0.11469825673487978</v>
       </c>
       <c r="G3">
         <f>Alkaline!B11</f>
@@ -4163,7 +4267,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" s="8">
         <f>PEM!B6/PEM!B5</f>
@@ -4183,7 +4287,7 @@
       </c>
       <c r="F4">
         <f>PEM!B12</f>
-        <v>0.11682954493601999</v>
+        <v>0.11469825673487978</v>
       </c>
       <c r="G4">
         <f>PEM!B11</f>
@@ -4192,7 +4296,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="9">
         <f>'HTSE future'!B7</f>
@@ -4212,7 +4316,7 @@
       </c>
       <c r="F5">
         <f>F2</f>
-        <v>0.10185220882315059</v>
+        <v>9.9589020191458474E-2</v>
       </c>
       <c r="G5">
         <f>G2</f>
@@ -4226,10 +4330,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C29FF039-2C41-394A-A2F3-20A4862B2BE3}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:I13"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4243,58 +4347,58 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
         <v>67</v>
-      </c>
-      <c r="I1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2">
-        <v>0.08</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
         <v>70</v>
       </c>
-      <c r="B3" t="s">
+      <c r="I3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" t="s">
         <v>71</v>
       </c>
-      <c r="I3" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>72</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>73</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>74</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>75</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>76</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>77</v>
-      </c>
-      <c r="P3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I4" s="11">
         <v>0.02</v>
@@ -4363,7 +4467,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I6" s="11">
         <v>0.06</v>
@@ -4399,7 +4503,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" t="str">
         <f>ANRs!B1</f>
@@ -4460,23 +4564,23 @@
       </c>
       <c r="B8" s="6">
         <f>((ANRs!B$13*1000*ANRs!B$5*ANRs!B$19+ANRs!B$14*1000*ANRs!B$5+(ANRs!B$15+ANRs!B$16)*ANRs!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!B$5))/('H2 recap'!$E2*ANRs!B$5)</f>
-        <v>3.9997371849327354</v>
+        <v>3.9088378808861468</v>
       </c>
       <c r="C8" s="6">
         <f>((ANRs!C$13*1000*ANRs!C$5*ANRs!C$19+ANRs!C$14*1000*ANRs!C$5+(ANRs!C$15+ANRs!C$16)*ANRs!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!C$5))/('H2 recap'!$E2*ANRs!C$5)</f>
-        <v>5.2301551867185276</v>
+        <v>5.1096907791073196</v>
       </c>
       <c r="D8" s="6">
         <f>((ANRs!D$13*1000*ANRs!D$5*ANRs!D$19+ANRs!D$14*1000*ANRs!D$5+(ANRs!D$15+ANRs!D$16)*ANRs!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!D$5))/('H2 recap'!$E2*ANRs!D$5)</f>
-        <v>3.6633754989260874</v>
+        <v>3.5870104900669899</v>
       </c>
       <c r="E8" s="6">
         <f>((ANRs!E$13*1000*ANRs!E$5*ANRs!E$19+ANRs!E$14*1000*ANRs!E$5+(ANRs!E$15+ANRs!E$16)*ANRs!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!E$5))/('H2 recap'!$E2*ANRs!E$5)</f>
-        <v>3.3156564060769256</v>
+        <v>3.2464833155404169</v>
       </c>
       <c r="F8" s="6">
         <f>((ANRs!F$13*1000*ANRs!F$5*ANRs!F$19+ANRs!F$14*1000*ANRs!F$5+(ANRs!F$15+ANRs!F$16)*ANRs!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*ANRs!F$5))/('H2 recap'!$E2*ANRs!F$5)</f>
-        <v>7.7850141120886134</v>
+        <v>7.6488856876447837</v>
       </c>
       <c r="I8" s="11">
         <v>0.1</v>
@@ -4517,23 +4621,23 @@
       </c>
       <c r="B9" s="6">
         <f>((ANRs!B$13*1000*ANRs!B$5*ANRs!B$19+ANRs!B$14*1000*ANRs!B$5+(ANRs!B$15+ANRs!B$16)*ANRs!B$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*ANRs!B$5))/('H2 recap'!$E3*ANRs!B$5)</f>
-        <v>4.2856135759729179</v>
+        <v>4.1860563903906485</v>
       </c>
       <c r="C9" s="6">
         <f>((ANRs!C$13*1000*ANRs!C$5*ANRs!C$19+ANRs!C$14*1000*ANRs!C$5+(ANRs!C$15+ANRs!C$16)*ANRs!C$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*ANRs!C$5))/('H2 recap'!$E3*ANRs!C$5)</f>
-        <v>5.5958629898418248</v>
+        <v>5.4648224713106774</v>
       </c>
       <c r="D9" s="6">
         <f>((ANRs!D$13*1000*ANRs!D$5*ANRs!D$19+ANRs!D$14*1000*ANRs!D$5+(ANRs!D$15+ANRs!D$16)*ANRs!D$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*ANRs!D$5))/('H2 recap'!$E3*ANRs!D$5)</f>
-        <v>3.9274282265237681</v>
+        <v>3.8433483435514812</v>
       </c>
       <c r="E9" s="6">
         <f>((ANRs!E$13*1000*ANRs!E$5*ANRs!E$19+ANRs!E$14*1000*ANRs!E$5+(ANRs!E$15+ANRs!E$16)*ANRs!E$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*ANRs!E$5))/('H2 recap'!$E3*ANRs!E$5)</f>
-        <v>3.5571485842108306</v>
+        <v>3.4807272422815783</v>
       </c>
       <c r="F9" s="6">
         <f>((ANRs!F$13*1000*ANRs!F$5*ANRs!F$19+ANRs!F$14*1000*ANRs!F$5+(ANRs!F$15+ANRs!F$16)*ANRs!F$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*ANRs!F$5))/('H2 recap'!$E3*ANRs!F$5)</f>
-        <v>8.3164850911321473</v>
+        <v>8.1687642502682714</v>
       </c>
       <c r="I9" s="11">
         <v>0.12</v>
@@ -4574,23 +4678,23 @@
       </c>
       <c r="B10" s="6">
         <f>((ANRs!B$13*1000*ANRs!B$5*ANRs!B$19+ANRs!B$14*1000*ANRs!B$5+(ANRs!B$15+ANRs!B$16)*ANRs!B$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*ANRs!B$5))/('H2 recap'!$E4*ANRs!B$5)</f>
-        <v>4.753375322827309</v>
+        <v>4.644401155916773</v>
       </c>
       <c r="C10" s="6">
         <f>((ANRs!C$13*1000*ANRs!C$5*ANRs!C$19+ANRs!C$14*1000*ANRs!C$5+(ANRs!C$15+ANRs!C$16)*ANRs!C$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*ANRs!C$5))/('H2 recap'!$E4*ANRs!C$5)</f>
-        <v>6.1430104364776845</v>
+        <v>6.0006454170337209</v>
       </c>
       <c r="D10" s="6">
         <f>((ANRs!D$13*1000*ANRs!D$5*ANRs!D$19+ANRs!D$14*1000*ANRs!D$5+(ANRs!D$15+ANRs!D$16)*ANRs!D$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*ANRs!D$5))/('H2 recap'!$E4*ANRs!D$5)</f>
-        <v>4.3734881551468288</v>
+        <v>4.280929033298527</v>
       </c>
       <c r="E10" s="6">
         <f>((ANRs!E$13*1000*ANRs!E$5*ANRs!E$19+ANRs!E$14*1000*ANRs!E$5+(ANRs!E$15+ANRs!E$16)*ANRs!E$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*ANRs!E$5))/('H2 recap'!$E4*ANRs!E$5)</f>
-        <v>3.9807739227408128</v>
+        <v>3.8963373594222714</v>
       </c>
       <c r="F10" s="6">
         <f>((ANRs!F$13*1000*ANRs!F$5*ANRs!F$19+ANRs!F$14*1000*ANRs!F$5+(ANRs!F$15+ANRs!F$16)*ANRs!F$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*ANRs!F$5))/('H2 recap'!$E4*ANRs!F$5)</f>
-        <v>9.0284702297873629</v>
+        <v>8.8684142567163953</v>
       </c>
       <c r="I10" s="11">
         <v>0.14000000000000001</v>
@@ -4631,23 +4735,23 @@
       </c>
       <c r="B11" s="6">
         <f>((ANRs!B$13*1000*ANRs!B$5*ANRs!B$19+ANRs!B$14*1000*ANRs!B$5+(ANRs!B$15+ANRs!B$16)*ANRs!B$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*ANRs!B$5))/('H2 recap'!$E5*ANRs!B$5)</f>
-        <v>2.9260599590265239</v>
+        <v>2.8571636747499065</v>
       </c>
       <c r="C11" s="6">
         <f>((ANRs!C$13*1000*ANRs!C$5*ANRs!C$19+ANRs!C$14*1000*ANRs!C$5+(ANRs!C$15+ANRs!C$16)*ANRs!C$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*ANRs!C$5))/('H2 recap'!$E5*ANRs!C$5)</f>
-        <v>3.8864778723139555</v>
+        <v>3.7945041826105261</v>
       </c>
       <c r="D11" s="6">
         <f>((ANRs!D$13*1000*ANRs!D$5*ANRs!D$19+ANRs!D$14*1000*ANRs!D$5+(ANRs!D$15+ANRs!D$16)*ANRs!D$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*ANRs!D$5))/('H2 recap'!$E5*ANRs!D$5)</f>
-        <v>2.6635087056187512</v>
+        <v>2.6059573443153137</v>
       </c>
       <c r="E11" s="6">
         <f>((ANRs!E$13*1000*ANRs!E$5*ANRs!E$19+ANRs!E$14*1000*ANRs!E$5+(ANRs!E$15+ANRs!E$16)*ANRs!E$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*ANRs!E$5))/('H2 recap'!$E5*ANRs!E$5)</f>
-        <v>2.3920922885314706</v>
+        <v>2.3401546675812215</v>
       </c>
       <c r="F11" s="6">
         <f>((ANRs!F$13*1000*ANRs!F$5*ANRs!F$19+ANRs!F$14*1000*ANRs!F$5+(ANRs!F$15+ANRs!F$16)*ANRs!F$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*ANRs!F$5))/('H2 recap'!$E5*ANRs!F$5)</f>
-        <v>5.8807044475806016</v>
+        <v>5.7765040167710984</v>
       </c>
       <c r="I11" s="11">
         <v>0.16</v>
@@ -4716,13 +4820,13 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
         <v>82</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>83</v>
-      </c>
-      <c r="C13" t="s">
-        <v>84</v>
       </c>
       <c r="I13" s="11">
         <v>0.2</v>
@@ -4758,20 +4862,20 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14">
         <f>ANRs!D13*ANRs!D5*1000*ANRs!D19+'H2 recap'!B2*ANRs!D5*'H2 recap'!F2</f>
-        <v>34800956.455252074</v>
+        <v>33628001.274567991</v>
       </c>
       <c r="C14">
         <f>ANRs!E13*ANRs!E5*1000*ANRs!E19+'H2 recap'!B4*'H2 recap'!F4*ANRs!E5</f>
-        <v>66209590.928097278</v>
+        <v>64185646.505351841</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15">
         <f>ANRs!D14*ANRs!D5*1000+'H2 recap'!C2*ANRs!D5</f>
@@ -4784,7 +4888,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16">
         <f>(ANRs!D15+ANRs!D16)*ANRs!D5*(365*24)+'H2 recap'!D2*ANRs!D5</f>
@@ -4797,7 +4901,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <f>'H2 recap'!E2*ANRs!D5</f>
@@ -4810,25 +4914,25 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18">
         <f>(B14+B15+B16)/B17</f>
-        <v>3.6633754989260878</v>
+        <v>3.5870104900669908</v>
       </c>
       <c r="C18">
         <f>(C14+C15+C16)/C17</f>
-        <v>3.9807739227408128</v>
+        <v>3.8963373594222714</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
-        <v>87</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" t="str">
         <f>'ANRs NOAK'!B1</f>
@@ -4857,24 +4961,24 @@
         <v>HTSE</v>
       </c>
       <c r="B22" s="6">
-        <f>(('ANRs NOAK'!B$13*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!B$5))/('H2 recap'!$E2*'ANRs NOAK'!B$5)</f>
-        <v>3.4407109650378396</v>
+        <f>(('ANRs NOAK'!C$27*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!B$5))/('H2 recap'!$E2*'ANRs NOAK'!B$5)</f>
+        <v>3.3208202468186583</v>
       </c>
       <c r="C22" s="6">
-        <f>(('ANRs NOAK'!C$13*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!C$5))/('H2 recap'!$E2*'ANRs NOAK'!C$5)</f>
-        <v>4.472667083879915</v>
+        <f>(('ANRs NOAK'!D$27*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!C$5))/('H2 recap'!$E2*'ANRs NOAK'!C$5)</f>
+        <v>4.312918917227254</v>
       </c>
       <c r="D22" s="6">
-        <f>(('ANRs NOAK'!D$13*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!D$5))/('H2 recap'!$E2*'ANRs NOAK'!D$5)</f>
-        <v>3.2019137466768046</v>
+        <f>(('ANRs NOAK'!E$27*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!D$5))/('H2 recap'!$E2*'ANRs NOAK'!D$5)</f>
+        <v>3.1016170718096538</v>
       </c>
       <c r="E22" s="6">
-        <f>(('ANRs NOAK'!E$13*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!E$5))/('H2 recap'!$E2*'ANRs NOAK'!E$5)</f>
-        <v>2.9024718955818902</v>
+        <f>(('ANRs NOAK'!F$27*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!E$5))/('H2 recap'!$E2*'ANRs NOAK'!E$5)</f>
+        <v>2.8118708239469039</v>
       </c>
       <c r="F22" s="6">
-        <f>(('ANRs NOAK'!F$13*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!F$5))/('H2 recap'!$E2*'ANRs NOAK'!F$5)</f>
-        <v>6.3970096991956451</v>
+        <f>(('ANRs NOAK'!G$27*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!F$5))/('H2 recap'!$E2*'ANRs NOAK'!F$5)</f>
+        <v>6.168408330352233</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.5">
@@ -4883,24 +4987,24 @@
         <v>Alkaline</v>
       </c>
       <c r="B23" s="6">
-        <f>(('ANRs NOAK'!B$13*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!B$5))/('H2 recap'!$E3*'ANRs NOAK'!B$5)</f>
-        <v>3.6903168752650592</v>
+        <f>(('ANRs NOAK'!C$27*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!B$5))/('H2 recap'!$E3*'ANRs NOAK'!B$5)</f>
+        <v>3.5598872679759079</v>
       </c>
       <c r="C23" s="6">
-        <f>(('ANRs NOAK'!C$13*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!C$5))/('H2 recap'!$E3*'ANRs NOAK'!C$5)</f>
-        <v>4.7892278940317174</v>
+        <f>(('ANRs NOAK'!D$27*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!C$5))/('H2 recap'!$E3*'ANRs NOAK'!C$5)</f>
+        <v>4.6163548257622473</v>
       </c>
       <c r="D23" s="6">
-        <f>(('ANRs NOAK'!D$13*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!D$5))/('H2 recap'!$E3*'ANRs NOAK'!D$5)</f>
-        <v>3.4360261261562512</v>
+        <f>(('ANRs NOAK'!E$27*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!D$5))/('H2 recap'!$E3*'ANRs NOAK'!D$5)</f>
+        <v>3.3264618538833779</v>
       </c>
       <c r="E23" s="6">
-        <f>(('ANRs NOAK'!E$13*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!E$5))/('H2 recap'!$E3*'ANRs NOAK'!E$5)</f>
-        <v>3.1171560272829444</v>
+        <f>(('ANRs NOAK'!F$27*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!E$5))/('H2 recap'!$E3*'ANRs NOAK'!E$5)</f>
+        <v>3.017916423889762</v>
       </c>
       <c r="F23" s="6">
-        <f>(('ANRs NOAK'!F$13*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!F$5))/('H2 recap'!$E3*'ANRs NOAK'!F$5)</f>
-        <v>6.8384248174682707</v>
+        <f>(('ANRs NOAK'!G$27*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!F$5))/('H2 recap'!$E3*'ANRs NOAK'!F$5)</f>
+        <v>6.5922312453679934</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.5">
@@ -4909,24 +5013,24 @@
         <v>PEM</v>
       </c>
       <c r="B24" s="6">
-        <f>(('ANRs NOAK'!B$13*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!B$5))/('H2 recap'!$E4*'ANRs NOAK'!B$5)</f>
-        <v>4.1220106455471504</v>
+        <f>(('ANRs NOAK'!C$27*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!B$5))/('H2 recap'!$E4*'ANRs NOAK'!B$5)</f>
+        <v>3.9802935513792574</v>
       </c>
       <c r="C24" s="6">
-        <f>(('ANRs NOAK'!C$13*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!C$5))/('H2 recap'!$E4*'ANRs NOAK'!C$5)</f>
-        <v>5.287502743686141</v>
+        <f>(('ANRs NOAK'!D$27*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!C$5))/('H2 recap'!$E4*'ANRs NOAK'!C$5)</f>
+        <v>5.1007706141373577</v>
       </c>
       <c r="D24" s="6">
-        <f>(('ANRs NOAK'!D$13*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!D$5))/('H2 recap'!$E4*'ANRs NOAK'!D$5)</f>
-        <v>3.8523128686982209</v>
+        <f>(('ANRs NOAK'!E$27*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!D$5))/('H2 recap'!$E4*'ANRs NOAK'!D$5)</f>
+        <v>3.7327253033740622</v>
       </c>
       <c r="E24" s="6">
-        <f>(('ANRs NOAK'!E$13*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!E$5))/('H2 recap'!$E4*'ANRs NOAK'!E$5)</f>
-        <v>3.5141229932461195</v>
+        <f>(('ANRs NOAK'!F$27*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!E$5))/('H2 recap'!$E4*'ANRs NOAK'!E$5)</f>
+        <v>3.4054856502690685</v>
       </c>
       <c r="F24" s="6">
-        <f>(('ANRs NOAK'!F$13*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!F$5))/('H2 recap'!$E4*'ANRs NOAK'!F$5)</f>
-        <v>7.4608568924838501</v>
+        <f>(('ANRs NOAK'!G$27*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!F$5))/('H2 recap'!$E4*'ANRs NOAK'!F$5)</f>
+        <v>7.1963618991662743</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.5">
@@ -4935,24 +5039,274 @@
         <v>HTSE future</v>
       </c>
       <c r="B25" s="6">
-        <f>(('ANRs NOAK'!B$13*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!B$5))/('H2 recap'!$E5*'ANRs NOAK'!B$5)</f>
-        <v>2.4897051634975433</v>
+        <f>(('ANRs NOAK'!C$27*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!B$5))/('H2 recap'!$E5*'ANRs NOAK'!B$5)</f>
+        <v>2.3981792741091006</v>
       </c>
       <c r="C25" s="6">
-        <f>(('ANRs NOAK'!C$13*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!C$5))/('H2 recap'!$E5*'ANRs NOAK'!C$5)</f>
-        <v>3.2952112117055794</v>
+        <f>(('ANRs NOAK'!D$27*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!C$5))/('H2 recap'!$E5*'ANRs NOAK'!C$5)</f>
+        <v>3.1725741004414121</v>
       </c>
       <c r="D25" s="6">
-        <f>(('ANRs NOAK'!D$13*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!D$5))/('H2 recap'!$E5*'ANRs NOAK'!D$5)</f>
-        <v>2.3033090559761287</v>
+        <f>(('ANRs NOAK'!E$27*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!D$5))/('H2 recap'!$E5*'ANRs NOAK'!D$5)</f>
+        <v>2.2270775382578893</v>
       </c>
       <c r="E25" s="6">
-        <f>(('ANRs NOAK'!E$13*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!E$5))/('H2 recap'!$E5*'ANRs NOAK'!E$5)</f>
-        <v>2.0695760340582887</v>
+        <f>(('ANRs NOAK'!F$27*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!E$5))/('H2 recap'!$E5*'ANRs NOAK'!E$5)</f>
+        <v>2.0009125387607094</v>
       </c>
       <c r="F25" s="6">
-        <f>(('ANRs NOAK'!F$13*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!F$5))/('H2 recap'!$E5*'ANRs NOAK'!F$5)</f>
-        <v>4.7972805217849421</v>
+        <f>(('ANRs NOAK'!G$27*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!F$5))/('H2 recap'!$E5*'ANRs NOAK'!F$5)</f>
+        <v>4.6208991962169996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="4">
+        <f>(('ANRs NOAK'!C$28*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!B$5))/('H2 recap'!$E2*'ANRs NOAK'!B$5)</f>
+        <v>2.7525661273641995</v>
+      </c>
+      <c r="C29" s="4">
+        <f>(('ANRs NOAK'!D$28*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!C$5))/('H2 recap'!$E2*'ANRs NOAK'!C$5)</f>
+        <v>3.5429268854461449</v>
+      </c>
+      <c r="D29" s="4">
+        <f>(('ANRs NOAK'!E$28*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!D$5))/('H2 recap'!$E2*'ANRs NOAK'!D$5)</f>
+        <v>2.6325379260486024</v>
+      </c>
+      <c r="E29" s="4">
+        <f>(('ANRs NOAK'!F$28*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!E$5))/('H2 recap'!$E2*'ANRs NOAK'!E$5)</f>
+        <v>2.3918658370113683</v>
+      </c>
+      <c r="F29" s="4">
+        <f>(('ANRs NOAK'!G$28*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!F$5))/('H2 recap'!$E2*'ANRs NOAK'!F$5)</f>
+        <v>4.7376904261609694</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="4">
+        <f>(('ANRs NOAK'!C$28*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!B$5))/('H2 recap'!$E3*'ANRs NOAK'!B$5)</f>
+        <v>2.9547639473944698</v>
+      </c>
+      <c r="C30" s="4">
+        <f>(('ANRs NOAK'!D$28*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!C$5))/('H2 recap'!$E3*'ANRs NOAK'!C$5)</f>
+        <v>3.7964045268714108</v>
+      </c>
+      <c r="D30" s="4">
+        <f>(('ANRs NOAK'!E$28*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!D$5))/('H2 recap'!$E3*'ANRs NOAK'!D$5)</f>
+        <v>2.8269481317990799</v>
+      </c>
+      <c r="E30" s="4">
+        <f>(('ANRs NOAK'!F$28*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!E$5))/('H2 recap'!$E3*'ANRs NOAK'!E$5)</f>
+        <v>2.5706608675214402</v>
+      </c>
+      <c r="F30" s="4">
+        <f>(('ANRs NOAK'!G$28*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!F$5))/('H2 recap'!$E3*'ANRs NOAK'!F$5)</f>
+        <v>5.0686861634059124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="4">
+        <f>(('ANRs NOAK'!C$28*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!B$5))/('H2 recap'!$E4*'ANRs NOAK'!B$5)</f>
+        <v>3.3385068766684727</v>
+      </c>
+      <c r="C31" s="4">
+        <f>(('ANRs NOAK'!D$28*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!C$5))/('H2 recap'!$E4*'ANRs NOAK'!C$5)</f>
+        <v>4.2311409736078405</v>
+      </c>
+      <c r="D31" s="4">
+        <f>(('ANRs NOAK'!E$28*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!D$5))/('H2 recap'!$E4*'ANRs NOAK'!D$5)</f>
+        <v>3.2029469263634804</v>
+      </c>
+      <c r="E31" s="4">
+        <f>(('ANRs NOAK'!F$28*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!E$5))/('H2 recap'!$E4*'ANRs NOAK'!E$5)</f>
+        <v>2.931131669014901</v>
+      </c>
+      <c r="F31" s="4">
+        <f>(('ANRs NOAK'!G$28*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!F$5))/('H2 recap'!$E4*'ANRs NOAK'!F$5)</f>
+        <v>5.5805079092970793</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="4">
+        <f>(('ANRs NOAK'!C$28*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!B$5))/('H2 recap'!$E5*'ANRs NOAK'!B$5)</f>
+        <v>1.9546215280168486</v>
+      </c>
+      <c r="C32" s="4">
+        <f>(('ANRs NOAK'!D$28*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!C$5))/('H2 recap'!$E5*'ANRs NOAK'!C$5)</f>
+        <v>2.5715473442188492</v>
+      </c>
+      <c r="D32" s="4">
+        <f>(('ANRs NOAK'!E$28*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!D$5))/('H2 recap'!$E5*'ANRs NOAK'!D$5)</f>
+        <v>1.860932038367104</v>
+      </c>
+      <c r="E32" s="4">
+        <f>(('ANRs NOAK'!F$28*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!E$5))/('H2 recap'!$E5*'ANRs NOAK'!E$5)</f>
+        <v>1.6730724774665087</v>
+      </c>
+      <c r="F32" s="4">
+        <f>(('ANRs NOAK'!G$28*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!F$5))/('H2 recap'!$E5*'ANRs NOAK'!F$5)</f>
+        <v>3.5041347291399316</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="4">
+        <f>(('ANRs NOAK'!C$29*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!B$5))/('H2 recap'!$E2*'ANRs NOAK'!B$5)</f>
+        <v>2.4487998075517132</v>
+      </c>
+      <c r="C36" s="4">
+        <f>(('ANRs NOAK'!D$29*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!C$5))/('H2 recap'!$E2*'ANRs NOAK'!C$5)</f>
+        <v>3.1313194060254319</v>
+      </c>
+      <c r="D36" s="4">
+        <f>(('ANRs NOAK'!E$29*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!D$5))/('H2 recap'!$E2*'ANRs NOAK'!D$5)</f>
+        <v>2.381786649585504</v>
+      </c>
+      <c r="E36" s="4">
+        <f>(('ANRs NOAK'!F$29*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!E$5))/('H2 recap'!$E2*'ANRs NOAK'!E$5)</f>
+        <v>2.1673476772366835</v>
+      </c>
+      <c r="F36" s="4">
+        <f>(('ANRs NOAK'!G$29*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B2*'H2 recap'!$F2+'H2 recap'!$C2+'H2 recap'!$D2)*'ANRs NOAK'!F$5))/('H2 recap'!$E2*'ANRs NOAK'!F$5)</f>
+        <v>3.9728848619474699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="4">
+        <f>(('ANRs NOAK'!C$29*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!B$5))/('H2 recap'!$E3*'ANRs NOAK'!B$5)</f>
+        <v>2.6312888016230609</v>
+      </c>
+      <c r="C37" s="4">
+        <f>(('ANRs NOAK'!D$29*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!C$5))/('H2 recap'!$E3*'ANRs NOAK'!C$5)</f>
+        <v>3.3580913212190948</v>
+      </c>
+      <c r="D37" s="4">
+        <f>(('ANRs NOAK'!E$29*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!D$5))/('H2 recap'!$E3*'ANRs NOAK'!D$5)</f>
+        <v>2.5599277269156895</v>
+      </c>
+      <c r="E37" s="4">
+        <f>(('ANRs NOAK'!F$29*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!E$5))/('H2 recap'!$E3*'ANRs NOAK'!E$5)</f>
+        <v>2.3315756242782899</v>
+      </c>
+      <c r="F37" s="4">
+        <f>(('ANRs NOAK'!G$29*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B3*'H2 recap'!$F3+'H2 recap'!$C3+'H2 recap'!$D3)*'ANRs NOAK'!F$5))/('H2 recap'!$E3*'ANRs NOAK'!F$5)</f>
+        <v>4.2542588380741808</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="4">
+        <f>(('ANRs NOAK'!C$29*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!B$5))/('H2 recap'!$E4*'ANRs NOAK'!B$5)</f>
+        <v>2.9954329426532671</v>
+      </c>
+      <c r="C38" s="4">
+        <f>(('ANRs NOAK'!D$29*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!C$5))/('H2 recap'!$E4*'ANRs NOAK'!C$5)</f>
+        <v>3.7662711443189432</v>
+      </c>
+      <c r="D38" s="4">
+        <f>(('ANRs NOAK'!E$29*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!D$5))/('H2 recap'!$E4*'ANRs NOAK'!D$5)</f>
+        <v>2.9197482263606842</v>
+      </c>
+      <c r="E38" s="4">
+        <f>(('ANRs NOAK'!F$29*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!E$5))/('H2 recap'!$E4*'ANRs NOAK'!E$5)</f>
+        <v>2.677560672798784</v>
+      </c>
+      <c r="F38" s="4">
+        <f>(('ANRs NOAK'!G$29*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B4*'H2 recap'!$F4+'H2 recap'!$C4+'H2 recap'!$D4)*'ANRs NOAK'!F$5))/('H2 recap'!$E4*'ANRs NOAK'!F$5)</f>
+        <v>4.7167358695481907</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="4">
+        <f>(('ANRs NOAK'!C$29*1000*'ANRs NOAK'!B$5*'ANRs NOAK'!B$19+'ANRs NOAK'!B$14*1000*'ANRs NOAK'!B$5+('ANRs NOAK'!B$15+'ANRs NOAK'!B$16)*'ANRs NOAK'!B$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!B$5))/('H2 recap'!$E5*'ANRs NOAK'!B$5)</f>
+        <v>1.7175129888229457</v>
+      </c>
+      <c r="C39" s="4">
+        <f>(('ANRs NOAK'!D$29*1000*'ANRs NOAK'!C$5*'ANRs NOAK'!C$19+'ANRs NOAK'!C$14*1000*'ANRs NOAK'!C$5+('ANRs NOAK'!C$15+'ANRs NOAK'!C$16)*'ANRs NOAK'!C$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!C$5))/('H2 recap'!$E5*'ANRs NOAK'!C$5)</f>
+        <v>2.2502620607582755</v>
+      </c>
+      <c r="D39" s="4">
+        <f>(('ANRs NOAK'!E$29*1000*'ANRs NOAK'!D$5*'ANRs NOAK'!D$19+'ANRs NOAK'!D$14*1000*'ANRs NOAK'!D$5+('ANRs NOAK'!D$15+'ANRs NOAK'!D$16)*'ANRs NOAK'!D$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!D$5))/('H2 recap'!$E5*'ANRs NOAK'!D$5)</f>
+        <v>1.6652050436829227</v>
+      </c>
+      <c r="E39" s="4">
+        <f>(('ANRs NOAK'!F$29*1000*'ANRs NOAK'!E$5*'ANRs NOAK'!E$19+'ANRs NOAK'!E$14*1000*'ANRs NOAK'!E$5+('ANRs NOAK'!E$15+'ANRs NOAK'!E$16)*'ANRs NOAK'!E$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!E$5))/('H2 recap'!$E5*'ANRs NOAK'!E$5)</f>
+        <v>1.4978220648482143</v>
+      </c>
+      <c r="F39" s="4">
+        <f>(('ANRs NOAK'!G$29*1000*'ANRs NOAK'!F$5*'ANRs NOAK'!F$19+'ANRs NOAK'!F$14*1000*'ANRs NOAK'!F$5+('ANRs NOAK'!F$15+'ANRs NOAK'!F$16)*'ANRs NOAK'!F$5*(365*24))+(('H2 recap'!$B5*'H2 recap'!$F5+'H2 recap'!$C5+'H2 recap'!$D5)*'ANRs NOAK'!F$5))/('H2 recap'!$E5*'ANRs NOAK'!F$5)</f>
+        <v>2.9071563340039162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>